<commit_message>
Modified the data and added the Location quest
</commit_message>
<xml_diff>
--- a/SampleData.xlsx
+++ b/SampleData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538349\Desktop\GDP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538361\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20415" windowHeight="7590" firstSheet="6" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Location" sheetId="5" r:id="rId6"/>
     <sheet name="Competition" sheetId="6" r:id="rId7"/>
     <sheet name="CompetitionTeam" sheetId="8" r:id="rId8"/>
+    <sheet name="LocationQuest" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="116">
   <si>
     <t>TeamName</t>
   </si>
@@ -361,13 +362,31 @@
   </si>
   <si>
     <t>police department</t>
+  </si>
+  <si>
+    <t>Player_ID</t>
+  </si>
+  <si>
+    <t>Team_ID</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>PlayerID</t>
+  </si>
+  <si>
+    <t>Competition_ID</t>
+  </si>
+  <si>
+    <t>LocationNumber</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -379,6 +398,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -405,10 +432,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -692,8 +720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -911,7 +939,249 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="28.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>100</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="2">
+        <v>44065</v>
+      </c>
+      <c r="E2" s="2">
+        <v>44067</v>
+      </c>
+      <c r="F2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>101</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="2">
+        <v>44065</v>
+      </c>
+      <c r="E3" s="2">
+        <v>44066</v>
+      </c>
+      <c r="F3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>102</v>
+      </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="2">
+        <v>44065</v>
+      </c>
+      <c r="E4" s="2">
+        <v>44067</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>103</v>
+      </c>
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="2">
+        <v>44065</v>
+      </c>
+      <c r="E5" s="2">
+        <v>44066</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>104</v>
+      </c>
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="2">
+        <v>44065</v>
+      </c>
+      <c r="E6" s="2">
+        <v>44067</v>
+      </c>
+      <c r="F6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>105</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="2">
+        <v>44065</v>
+      </c>
+      <c r="E7" s="2">
+        <v>44067</v>
+      </c>
+      <c r="F7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>106</v>
+      </c>
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="2">
+        <v>44065</v>
+      </c>
+      <c r="E8" s="2">
+        <v>44067</v>
+      </c>
+      <c r="F8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>107</v>
+      </c>
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="2">
+        <v>44065</v>
+      </c>
+      <c r="E9" s="2">
+        <v>44066</v>
+      </c>
+      <c r="F9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>108</v>
+      </c>
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="2">
+        <v>44065</v>
+      </c>
+      <c r="E10" s="2">
+        <v>44067</v>
+      </c>
+      <c r="F10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>109</v>
+      </c>
+      <c r="B11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="2">
+        <v>44065</v>
+      </c>
+      <c r="E11" s="2">
+        <v>44067</v>
+      </c>
+      <c r="F11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
@@ -919,269 +1189,128 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>44</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>10</v>
       </c>
       <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="2">
-        <v>44065</v>
-      </c>
-      <c r="D2" s="2">
-        <v>44067</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="2">
-        <v>44065</v>
-      </c>
-      <c r="D3" s="2">
-        <v>44066</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" s="2">
-        <v>44065</v>
-      </c>
-      <c r="D4" s="2">
-        <v>44067</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5" s="2">
-        <v>44065</v>
-      </c>
-      <c r="D5" s="2">
-        <v>44066</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C6" s="2">
-        <v>44065</v>
-      </c>
-      <c r="D6" s="2">
-        <v>44067</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C7">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="2">
-        <v>44065</v>
-      </c>
-      <c r="D7" s="2">
-        <v>44067</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C8" s="2">
-        <v>44065</v>
-      </c>
-      <c r="D8" s="2">
-        <v>44067</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>51</v>
+      <c r="C8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>17</v>
       </c>
       <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="2">
-        <v>44065</v>
-      </c>
-      <c r="D9" s="2">
-        <v>44066</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="2">
-        <v>44065</v>
-      </c>
-      <c r="D10" s="2">
-        <v>44067</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>53</v>
+      <c r="C10">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" s="2">
-        <v>44065</v>
-      </c>
-      <c r="D11" s="2">
-        <v>44067</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B3">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B5">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B6">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B7">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
         <v>67</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>37</v>
       </c>
     </row>
@@ -1192,135 +1321,201 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>100</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2">
         <v>44058</v>
       </c>
-      <c r="B2" s="2">
+      <c r="D2" s="2">
         <v>44059</v>
       </c>
-      <c r="D2" s="2">
+      <c r="F2" s="2">
         <v>44067</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>101</v>
+      </c>
+      <c r="B3">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2">
         <v>44058</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2">
+      <c r="D3" s="2"/>
+      <c r="E3" s="2">
         <v>44061</v>
       </c>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>102</v>
+      </c>
+      <c r="B4">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2">
         <v>44058</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2">
         <v>44061</v>
       </c>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>103</v>
+      </c>
+      <c r="B5">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2">
         <v>44058</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2">
+      <c r="D5" s="2"/>
+      <c r="E5" s="2">
         <v>44061</v>
       </c>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>104</v>
+      </c>
+      <c r="B6">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2">
         <v>44059</v>
       </c>
-      <c r="B6" s="2">
+      <c r="D6" s="2">
         <v>44060</v>
       </c>
-      <c r="D6" s="2">
+      <c r="F6" s="2">
         <v>44067</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>105</v>
+      </c>
+      <c r="B7">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2">
         <v>44060</v>
       </c>
-      <c r="B7" s="2">
+      <c r="D7" s="2">
         <v>44061</v>
       </c>
-      <c r="D7" s="2">
+      <c r="F7" s="2">
         <v>44067</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>106</v>
+      </c>
+      <c r="B8">
+        <v>16</v>
+      </c>
+      <c r="C8" s="2">
         <v>44059</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2">
         <v>44062</v>
       </c>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>107</v>
+      </c>
+      <c r="B9">
+        <v>17</v>
+      </c>
+      <c r="C9" s="2">
         <v>44060</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2">
         <v>44063</v>
       </c>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>108</v>
+      </c>
+      <c r="B10">
+        <v>18</v>
+      </c>
+      <c r="C10" s="2">
         <v>44061</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2">
         <v>44064</v>
       </c>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>109</v>
+      </c>
+      <c r="B11">
+        <v>19</v>
+      </c>
+      <c r="C11" s="2">
         <v>44062</v>
       </c>
-      <c r="B11" s="2">
+      <c r="D11" s="2">
         <v>44063</v>
       </c>
-      <c r="D11" s="2">
+      <c r="F11" s="2">
         <v>44067</v>
       </c>
     </row>
@@ -1333,8 +1528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1346,16 +1541,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1501,6 +1696,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1509,7 +1705,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1520,13 +1716,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1647,205 +1843,240 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="5" max="6" width="11" customWidth="1"/>
+    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="6" max="7" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>111</v>
+      </c>
+      <c r="B2" t="s">
         <v>80</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="2">
+      <c r="D2" s="2">
         <v>44058</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="2">
         <v>44059</v>
       </c>
-      <c r="E2" s="2">
-        <v>44065</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="F2" s="2">
+        <v>44065</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>222</v>
+      </c>
+      <c r="B3" t="s">
         <v>81</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D3" s="2">
         <v>44060</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>44061</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>44067</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>333</v>
+      </c>
+      <c r="B4" t="s">
         <v>82</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D4" s="2">
         <v>44061</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="2">
         <v>44062</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>44066</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>444</v>
+      </c>
+      <c r="B5" t="s">
         <v>83</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>59</v>
-      </c>
-      <c r="C5" s="2">
-        <v>44062</v>
       </c>
       <c r="D5" s="2">
         <v>44062</v>
       </c>
       <c r="E5" s="2">
+        <v>44062</v>
+      </c>
+      <c r="F5" s="2">
         <v>44067</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>555</v>
+      </c>
+      <c r="B6" t="s">
         <v>84</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="2">
+      <c r="D6" s="2">
         <v>44059</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E6" s="2">
         <v>44060</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F6" s="2">
         <v>44066</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>666</v>
+      </c>
+      <c r="B7" t="s">
         <v>85</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>57</v>
-      </c>
-      <c r="C7" s="2">
-        <v>44063</v>
       </c>
       <c r="D7" s="2">
         <v>44063</v>
       </c>
       <c r="E7" s="2">
+        <v>44063</v>
+      </c>
+      <c r="F7" s="2">
         <v>44067</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>777</v>
+      </c>
+      <c r="B8" t="s">
         <v>86</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="2">
+      <c r="D8" s="2">
         <v>44060</v>
       </c>
-      <c r="D8" s="2">
+      <c r="E8" s="2">
         <v>44061</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F8" s="2">
         <v>44067</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>888</v>
+      </c>
+      <c r="B9" t="s">
         <v>87</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="2">
+      <c r="D9" s="2">
         <v>44061</v>
       </c>
-      <c r="D9" s="2">
+      <c r="E9" s="2">
         <v>44062</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F9" s="2">
         <v>44066</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>999</v>
+      </c>
+      <c r="B10" t="s">
         <v>88</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="2">
+      <c r="D10" s="2">
         <v>44064</v>
       </c>
-      <c r="D10" s="2">
-        <v>44065</v>
-      </c>
       <c r="E10" s="2">
+        <v>44065</v>
+      </c>
+      <c r="F10" s="2">
         <v>44068</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>234</v>
+      </c>
+      <c r="B11" t="s">
         <v>89</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>67</v>
       </c>
-      <c r="C11" s="2">
-        <v>44065</v>
-      </c>
       <c r="D11" s="2">
+        <v>44065</v>
+      </c>
+      <c r="E11" s="2">
         <v>44066</v>
       </c>
-      <c r="E11" s="2">
+      <c r="F11" s="2">
         <v>44069</v>
       </c>
     </row>
@@ -1858,8 +2089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1869,13 +2100,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1884,7 +2115,7 @@
         <v>111</v>
       </c>
       <c r="B2">
-        <v>1111</v>
+        <v>100</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -1895,7 +2126,7 @@
         <v>222</v>
       </c>
       <c r="B3">
-        <v>1234</v>
+        <v>101</v>
       </c>
       <c r="C3">
         <v>110</v>
@@ -1906,7 +2137,7 @@
         <v>333</v>
       </c>
       <c r="B4">
-        <v>2345</v>
+        <v>102</v>
       </c>
       <c r="C4">
         <v>120</v>
@@ -1917,7 +2148,7 @@
         <v>444</v>
       </c>
       <c r="B5">
-        <v>3456</v>
+        <v>103</v>
       </c>
       <c r="C5">
         <v>130</v>
@@ -1928,7 +2159,7 @@
         <v>555</v>
       </c>
       <c r="B6">
-        <v>4567</v>
+        <v>104</v>
       </c>
       <c r="C6">
         <v>140</v>
@@ -1939,7 +2170,7 @@
         <v>666</v>
       </c>
       <c r="B7">
-        <v>5678</v>
+        <v>105</v>
       </c>
       <c r="C7">
         <v>150</v>
@@ -1950,7 +2181,7 @@
         <v>777</v>
       </c>
       <c r="B8">
-        <v>6789</v>
+        <v>106</v>
       </c>
       <c r="C8">
         <v>160</v>
@@ -1961,7 +2192,7 @@
         <v>888</v>
       </c>
       <c r="B9">
-        <v>4444</v>
+        <v>107</v>
       </c>
       <c r="C9">
         <v>170</v>
@@ -1972,7 +2203,7 @@
         <v>999</v>
       </c>
       <c r="B10">
-        <v>5555</v>
+        <v>108</v>
       </c>
       <c r="C10">
         <v>180</v>
@@ -1983,10 +2214,117 @@
         <v>234</v>
       </c>
       <c r="B11">
-        <v>4557</v>
+        <v>109</v>
       </c>
       <c r="C11">
         <v>190</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updation of sample data
</commit_message>
<xml_diff>
--- a/SampleData.xlsx
+++ b/SampleData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -947,8 +947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1027,7 +1027,7 @@
         <v>31</v>
       </c>
       <c r="G3">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1050,7 +1050,7 @@
         <v>27</v>
       </c>
       <c r="G4">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1096,7 +1096,7 @@
         <v>28</v>
       </c>
       <c r="G6">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1119,7 +1119,7 @@
         <v>32</v>
       </c>
       <c r="G7">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1142,7 +1142,7 @@
         <v>42</v>
       </c>
       <c r="G8">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1165,7 +1165,7 @@
         <v>60</v>
       </c>
       <c r="G9">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1188,7 +1188,7 @@
         <v>40</v>
       </c>
       <c r="G10">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1211,7 +1211,7 @@
         <v>63</v>
       </c>
       <c r="G11">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1223,7 +1223,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -1273,7 +1273,7 @@
         <v>27</v>
       </c>
       <c r="D3">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1287,7 +1287,7 @@
         <v>37</v>
       </c>
       <c r="D4">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1301,7 +1301,7 @@
         <v>45</v>
       </c>
       <c r="D5">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1315,7 +1315,7 @@
         <v>28</v>
       </c>
       <c r="D6">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1329,7 +1329,7 @@
         <v>29</v>
       </c>
       <c r="D7">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1343,7 +1343,7 @@
         <v>30</v>
       </c>
       <c r="D8">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1357,7 +1357,7 @@
         <v>34</v>
       </c>
       <c r="D9">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1371,7 +1371,7 @@
         <v>28</v>
       </c>
       <c r="D10">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1385,7 +1385,7 @@
         <v>37</v>
       </c>
       <c r="D11">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1919,7 +1919,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated sample data according to the er diagram
</commit_message>
<xml_diff>
--- a/SampleData.xlsx
+++ b/SampleData.xlsx
@@ -951,7 +951,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1007,7 +1007,7 @@
         <v>30</v>
       </c>
       <c r="G2">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1030,7 +1030,7 @@
         <v>31</v>
       </c>
       <c r="G3">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1053,7 +1053,7 @@
         <v>27</v>
       </c>
       <c r="G4">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1076,7 +1076,7 @@
         <v>29</v>
       </c>
       <c r="G5">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1099,7 +1099,7 @@
         <v>28</v>
       </c>
       <c r="G6">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1122,7 +1122,7 @@
         <v>32</v>
       </c>
       <c r="G7">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1145,7 +1145,7 @@
         <v>42</v>
       </c>
       <c r="G8">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1168,7 +1168,7 @@
         <v>60</v>
       </c>
       <c r="G9">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1191,7 +1191,7 @@
         <v>40</v>
       </c>
       <c r="G10">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1214,7 +1214,7 @@
         <v>118</v>
       </c>
       <c r="G11">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated sample data in excel sheet
</commit_message>
<xml_diff>
--- a/SampleData.xlsx
+++ b/SampleData.xlsx
@@ -951,7 +951,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1007,7 +1007,7 @@
         <v>30</v>
       </c>
       <c r="G2">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1030,7 +1030,7 @@
         <v>31</v>
       </c>
       <c r="G3">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1053,7 +1053,7 @@
         <v>27</v>
       </c>
       <c r="G4">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1076,7 +1076,7 @@
         <v>29</v>
       </c>
       <c r="G5">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1099,7 +1099,7 @@
         <v>28</v>
       </c>
       <c r="G6">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1122,7 +1122,7 @@
         <v>32</v>
       </c>
       <c r="G7">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1145,7 +1145,7 @@
         <v>42</v>
       </c>
       <c r="G8">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1168,7 +1168,7 @@
         <v>60</v>
       </c>
       <c r="G9">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1191,7 +1191,7 @@
         <v>40</v>
       </c>
       <c r="G10">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1214,7 +1214,7 @@
         <v>118</v>
       </c>
       <c r="G11">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>